<commit_message>
reduced number of line in main.py
</commit_message>
<xml_diff>
--- a/brocode.xlsx
+++ b/brocode.xlsx
@@ -9,14 +9,14 @@
     <sheet name="template" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="13">
+  <fonts count="11">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -67,40 +67,31 @@
     <font>
       <name val="Calibri"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="14"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <b val="1"/>
-      <sz val="14"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
       <color rgb="FFFF0000"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
       <name val="Calibri"/>
+      <family val="2"/>
       <b val="1"/>
+      <color rgb="FF000000"/>
       <sz val="14"/>
     </font>
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <b val="1"/>
-      <sz val="14"/>
+      <color theme="1"/>
+      <sz val="16"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b val="1"/>
       <sz val="14"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -121,17 +112,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF9C2C95"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="009c2c95"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -239,68 +224,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -314,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
@@ -328,12 +261,10 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -358,82 +289,48 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="4" fillId="2" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="2" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="3" fontId="6" fillId="2" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="2" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="3" fontId="6" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="3" fontId="7" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="3" fontId="10" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="3" fontId="7" fillId="2" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="2" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="2" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="2" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
@@ -457,12 +354,13 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -833,310 +731,310 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="61" customWidth="1" style="65" min="1" max="1"/>
+    <col width="61" customWidth="1" style="49" min="1" max="1"/>
     <col width="5.28515625" customWidth="1" style="4" min="2" max="2"/>
-    <col width="6.140625" customWidth="1" style="63" min="3" max="3"/>
-    <col width="27.28515625" customWidth="1" style="63" min="4" max="4"/>
-    <col width="14.5703125" bestFit="1" customWidth="1" style="65" min="5" max="5"/>
-    <col width="25" bestFit="1" customWidth="1" style="65" min="6" max="6"/>
-    <col width="21.140625" bestFit="1" customWidth="1" style="65" min="7" max="7"/>
-    <col width="4" customWidth="1" style="65" min="8" max="8"/>
-    <col width="15.7109375" bestFit="1" customWidth="1" style="65" min="9" max="9"/>
-    <col width="14" bestFit="1" customWidth="1" style="65" min="10" max="10"/>
+    <col width="6.140625" customWidth="1" style="47" min="3" max="3"/>
+    <col width="27.28515625" customWidth="1" style="47" min="4" max="4"/>
+    <col width="14.5703125" bestFit="1" customWidth="1" style="49" min="5" max="5"/>
+    <col width="25" customWidth="1" style="49" min="6" max="6"/>
+    <col width="21.140625" bestFit="1" customWidth="1" style="49" min="7" max="7"/>
+    <col width="4" customWidth="1" style="49" min="8" max="8"/>
+    <col width="15.7109375" bestFit="1" customWidth="1" style="49" min="9" max="9"/>
+    <col width="14" bestFit="1" customWidth="1" style="49" min="10" max="10"/>
   </cols>
   <sheetData>
-    <row r="1" ht="33.75" customHeight="1" s="65">
-      <c r="B1" s="64" t="inlineStr">
+    <row r="1" ht="33.75" customHeight="1" s="49">
+      <c r="B1" s="48" t="inlineStr">
         <is>
           <t>Mount Care International Pvt Ltd.</t>
         </is>
       </c>
       <c r="J1" s="1" t="n"/>
     </row>
-    <row r="2" hidden="1" ht="33.75" customHeight="1" s="65">
+    <row r="2" hidden="1" ht="33.75" customHeight="1" s="49">
       <c r="B2" s="6" t="n"/>
-      <c r="C2" s="7" t="n"/>
-      <c r="D2" s="7" t="n"/>
-      <c r="E2" s="8" t="n"/>
-      <c r="F2" s="8" t="n"/>
-      <c r="G2" s="8" t="n"/>
-      <c r="H2" s="8" t="n"/>
+      <c r="C2" s="18" t="n"/>
+      <c r="D2" s="18" t="n"/>
+      <c r="E2" s="19" t="n"/>
+      <c r="F2" s="19" t="n"/>
+      <c r="G2" s="19" t="n"/>
+      <c r="H2" s="19" t="n"/>
       <c r="J2" s="1" t="n"/>
     </row>
-    <row r="3" ht="32.25" customHeight="1" s="65">
-      <c r="B3" s="66" t="inlineStr">
+    <row r="3" ht="32.25" customHeight="1" s="49">
+      <c r="B3" s="50" t="inlineStr">
         <is>
           <t>Gokarneshwor - 4, Kathmandu</t>
         </is>
       </c>
       <c r="J3" s="2" t="n"/>
     </row>
-    <row r="4" ht="32.25" customHeight="1" s="65">
-      <c r="B4" s="66" t="inlineStr">
+    <row r="4" ht="32.25" customHeight="1" s="49">
+      <c r="B4" s="50" t="inlineStr">
         <is>
           <t>Phone Number : 9851177355, 9823681553</t>
         </is>
       </c>
       <c r="J4" s="2" t="n"/>
     </row>
-    <row r="5" ht="32.25" customHeight="1" s="65">
-      <c r="B5" s="67" t="inlineStr">
+    <row r="5" ht="32.25" customHeight="1" s="49">
+      <c r="B5" s="51" t="inlineStr">
         <is>
           <t>Email - mountcareintl@gmail.com</t>
         </is>
       </c>
       <c r="J5" s="2" t="n"/>
     </row>
-    <row r="6" ht="28.5" customHeight="1" s="65">
+    <row r="6" ht="28.5" customHeight="1" s="49">
       <c r="A6" s="2" t="n"/>
-      <c r="B6" s="9" t="n"/>
-      <c r="C6" s="9" t="n"/>
-      <c r="D6" s="9" t="n"/>
-      <c r="E6" s="10" t="n"/>
-      <c r="F6" s="10" t="n"/>
-      <c r="G6" s="10" t="n"/>
-      <c r="H6" s="10" t="n"/>
+      <c r="B6" s="7" t="n"/>
+      <c r="C6" s="7" t="n"/>
+      <c r="D6" s="7" t="n"/>
+      <c r="E6" s="8" t="n"/>
+      <c r="F6" s="8" t="n"/>
+      <c r="G6" s="8" t="n"/>
+      <c r="H6" s="8" t="n"/>
       <c r="I6" s="2" t="n"/>
       <c r="J6" s="2" t="n"/>
     </row>
-    <row r="7" ht="23.25" customHeight="1" s="65">
+    <row r="7" ht="23.25" customHeight="1" s="49">
       <c r="B7" s="6" t="n"/>
-      <c r="C7" s="60" t="inlineStr">
+      <c r="C7" s="44" t="inlineStr">
         <is>
           <t xml:space="preserve"> Bill No                      : </t>
         </is>
       </c>
-      <c r="D7" s="61" t="n"/>
-      <c r="E7" s="11" t="n">
-        <v>74</v>
-      </c>
-      <c r="F7" s="12" t="inlineStr">
+      <c r="D7" s="45" t="n"/>
+      <c r="E7" s="9" t="n">
+        <v>163</v>
+      </c>
+      <c r="F7" s="10" t="inlineStr">
         <is>
           <t>Date :</t>
         </is>
       </c>
-      <c r="G7" s="13" t="inlineStr">
-        <is>
-          <t>2082-02-18</t>
-        </is>
-      </c>
-      <c r="H7" s="8" t="n"/>
-    </row>
-    <row r="8" ht="23.25" customHeight="1" s="65">
+      <c r="G7" s="11" t="inlineStr">
+        <is>
+          <t>2082-02-19</t>
+        </is>
+      </c>
+      <c r="H7" s="19" t="n"/>
+    </row>
+    <row r="8" ht="23.25" customHeight="1" s="49">
       <c r="B8" s="6" t="n"/>
-      <c r="C8" s="62" t="inlineStr">
+      <c r="C8" s="46" t="inlineStr">
         <is>
           <t xml:space="preserve"> Buyer's Name         :</t>
         </is>
       </c>
-      <c r="E8" s="14" t="inlineStr">
+      <c r="E8" s="12" t="inlineStr">
         <is>
           <t>ss</t>
         </is>
       </c>
-      <c r="F8" s="15" t="n"/>
-      <c r="G8" s="16" t="n"/>
-      <c r="H8" s="8" t="n"/>
+      <c r="F8" s="13" t="n"/>
+      <c r="G8" s="14" t="n"/>
+      <c r="H8" s="19" t="n"/>
       <c r="J8" s="3" t="n"/>
       <c r="K8" s="5" t="n"/>
-      <c r="L8" s="22" t="n"/>
-    </row>
-    <row r="9" ht="23.25" customHeight="1" s="65">
+      <c r="L8" s="17" t="n"/>
+    </row>
+    <row r="9" ht="23.25" customHeight="1" s="49">
       <c r="B9" s="6" t="n"/>
-      <c r="C9" s="62" t="inlineStr">
+      <c r="C9" s="46" t="inlineStr">
         <is>
           <t xml:space="preserve"> Customer Id            :</t>
         </is>
       </c>
-      <c r="E9" s="17" t="inlineStr">
+      <c r="E9" s="15" t="inlineStr">
         <is>
           <t>ss</t>
         </is>
       </c>
-      <c r="F9" s="18" t="n"/>
-      <c r="G9" s="16" t="n"/>
-      <c r="H9" s="8" t="n"/>
+      <c r="F9" s="16" t="n"/>
+      <c r="G9" s="14" t="n"/>
+      <c r="H9" s="19" t="n"/>
       <c r="J9" s="3" t="n"/>
     </row>
-    <row r="10" ht="23.25" customHeight="1" s="65">
+    <row r="10" ht="23.25" customHeight="1" s="49">
       <c r="B10" s="6" t="n"/>
-      <c r="C10" s="62" t="inlineStr">
+      <c r="C10" s="46" t="inlineStr">
         <is>
           <t xml:space="preserve"> Address                   :</t>
         </is>
       </c>
-      <c r="E10" s="14" t="inlineStr">
+      <c r="E10" s="12" t="inlineStr">
         <is>
           <t>ss</t>
         </is>
       </c>
-      <c r="F10" s="15" t="n"/>
-      <c r="G10" s="16" t="n"/>
-      <c r="H10" s="8" t="n"/>
+      <c r="F10" s="13" t="n"/>
+      <c r="G10" s="14" t="n"/>
+      <c r="H10" s="19" t="n"/>
       <c r="J10" s="3" t="n"/>
     </row>
-    <row r="11" ht="18.75" customHeight="1" s="65">
+    <row r="11" ht="18.75" customHeight="1" s="49">
       <c r="B11" s="6" t="n"/>
       <c r="C11" s="27" t="n"/>
-      <c r="D11" s="37" t="n"/>
-      <c r="E11" s="35" t="n"/>
-      <c r="F11" s="37" t="n"/>
-      <c r="G11" s="38" t="n"/>
-      <c r="H11" s="8" t="n"/>
-    </row>
-    <row r="12" ht="21" customHeight="1" s="65">
-      <c r="B12" s="6" t="n"/>
-      <c r="C12" s="23" t="inlineStr">
+      <c r="D11" s="26" t="n"/>
+      <c r="E11" s="21" t="n"/>
+      <c r="F11" s="26" t="n"/>
+      <c r="G11" s="29" t="n"/>
+      <c r="H11" s="19" t="n"/>
+    </row>
+    <row r="12" ht="21" customHeight="1" s="49">
+      <c r="B12" s="21" t="n"/>
+      <c r="C12" s="22" t="inlineStr">
         <is>
           <t>S.N</t>
         </is>
       </c>
-      <c r="D12" s="24" t="inlineStr">
+      <c r="D12" s="22" t="inlineStr">
         <is>
           <t>Particulars</t>
         </is>
       </c>
-      <c r="E12" s="25" t="inlineStr">
+      <c r="E12" s="23" t="inlineStr">
         <is>
           <t>Qty.</t>
         </is>
       </c>
-      <c r="F12" s="25" t="inlineStr">
+      <c r="F12" s="23" t="inlineStr">
         <is>
           <t>Rate</t>
         </is>
       </c>
-      <c r="G12" s="26" t="inlineStr">
+      <c r="G12" s="23" t="inlineStr">
         <is>
           <t>Amount</t>
         </is>
       </c>
-      <c r="H12" s="8" t="n"/>
-    </row>
-    <row r="13" ht="21" customHeight="1" s="65">
-      <c r="B13" s="35" t="n"/>
-      <c r="C13" s="62" t="n"/>
-      <c r="D13" s="39" t="n"/>
-      <c r="E13" s="40" t="n"/>
-      <c r="F13" s="30" t="n"/>
-      <c r="G13" s="13" t="n"/>
-      <c r="H13" s="31" t="n"/>
-    </row>
-    <row r="14" ht="18.75" customHeight="1" s="65">
-      <c r="B14" s="6" t="n"/>
+      <c r="H12" s="20" t="n"/>
+    </row>
+    <row r="13" ht="21" customHeight="1" s="49">
+      <c r="B13" s="25" t="n"/>
+      <c r="C13" s="27" t="n"/>
+      <c r="D13" s="25" t="n"/>
+      <c r="E13" s="26" t="n"/>
+      <c r="F13" s="25" t="n"/>
+      <c r="G13" s="29" t="n"/>
+      <c r="H13" s="24" t="n"/>
+    </row>
+    <row r="14" ht="18.75" customHeight="1" s="49">
+      <c r="B14" s="25" t="n"/>
       <c r="C14" s="27" t="n"/>
-      <c r="D14" s="41" t="n"/>
-      <c r="E14" s="42" t="n"/>
+      <c r="D14" s="25" t="n"/>
+      <c r="E14" s="26" t="n"/>
       <c r="F14" s="36" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="G14" s="28" t="inlineStr">
-        <is>
-          <t>Rs 47575.0</t>
-        </is>
-      </c>
-      <c r="H14" s="8" t="n"/>
-    </row>
-    <row r="15" ht="18.75" customHeight="1" s="65">
-      <c r="B15" s="6" t="n"/>
+      <c r="G14" s="38" t="inlineStr">
+        <is>
+          <t>Rs 46420.0</t>
+        </is>
+      </c>
+      <c r="H14" s="24" t="n"/>
+    </row>
+    <row r="15" ht="18.75" customHeight="1" s="49">
+      <c r="B15" s="25" t="n"/>
       <c r="C15" s="27" t="n"/>
-      <c r="D15" s="37" t="n"/>
-      <c r="E15" s="35" t="n"/>
+      <c r="D15" s="25" t="n"/>
+      <c r="E15" s="26" t="n"/>
       <c r="F15" s="36" t="inlineStr">
         <is>
           <t>Discount</t>
         </is>
       </c>
-      <c r="G15" s="28" t="inlineStr">
-        <is>
-          <t>Rs 4757.5</t>
-        </is>
-      </c>
-      <c r="H15" s="8" t="n"/>
-    </row>
-    <row r="16" ht="18.75" customHeight="1" s="65">
-      <c r="B16" s="6" t="n"/>
-      <c r="C16" s="19" t="n"/>
-      <c r="D16" s="20" t="n"/>
-      <c r="E16" s="21" t="n"/>
-      <c r="F16" s="32" t="inlineStr">
+      <c r="G15" s="38" t="inlineStr">
+        <is>
+          <t>Rs 4642.0</t>
+        </is>
+      </c>
+      <c r="H15" s="24" t="n"/>
+    </row>
+    <row r="16" ht="18.75" customHeight="1" s="49">
+      <c r="B16" s="25" t="n"/>
+      <c r="C16" s="28" t="n"/>
+      <c r="D16" s="30" t="n"/>
+      <c r="E16" s="32" t="n"/>
+      <c r="F16" s="37" t="inlineStr">
         <is>
           <t>Grand Total</t>
         </is>
       </c>
-      <c r="G16" s="33" t="inlineStr">
-        <is>
-          <t>Rs 42817.5</t>
-        </is>
-      </c>
-      <c r="H16" s="8" t="n"/>
-    </row>
-    <row r="17" ht="21" customHeight="1" s="65">
-      <c r="B17" s="35" t="n"/>
-      <c r="C17" s="34" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Amount in words: </t>
-        </is>
-      </c>
-      <c r="D17" s="43" t="n"/>
-      <c r="E17" s="56" t="inlineStr">
-        <is>
-          <t>Forty two thousand eight hundred and</t>
-        </is>
-      </c>
-      <c r="F17" s="54" t="n"/>
-      <c r="G17" s="55" t="n"/>
-      <c r="H17" s="31" t="n"/>
-    </row>
-    <row r="18" ht="18.75" customHeight="1" s="65">
+      <c r="G16" s="39" t="inlineStr">
+        <is>
+          <t>Rs 41778.0</t>
+        </is>
+      </c>
+      <c r="H16" s="24" t="n"/>
+    </row>
+    <row r="17" ht="21" customHeight="1" s="49">
+      <c r="B17" s="25" t="n"/>
+      <c r="C17" s="46" t="inlineStr">
+        <is>
+          <t>Amount in words:</t>
+        </is>
+      </c>
+      <c r="D17" s="25" t="n"/>
+      <c r="E17" s="40" t="inlineStr">
+        <is>
+          <t>Forty one thousand seven hundred and</t>
+        </is>
+      </c>
+      <c r="F17" s="30" t="n"/>
+      <c r="G17" s="31" t="n"/>
+      <c r="H17" s="24" t="n"/>
+    </row>
+    <row r="18" ht="18.75" customHeight="1" s="49">
       <c r="B18" s="6" t="n"/>
-      <c r="C18" s="19" t="n"/>
-      <c r="D18" s="29" t="n"/>
-      <c r="E18" s="56">
+      <c r="C18" s="28" t="n"/>
+      <c r="D18" s="32" t="n"/>
+      <c r="E18" s="52">
         <f>""</f>
         <v/>
       </c>
-      <c r="F18" s="49" t="n"/>
-      <c r="G18" s="50" t="n"/>
-      <c r="H18" s="8" t="n"/>
-    </row>
-    <row r="19" ht="18.75" customHeight="1" s="65">
-      <c r="B19" s="44" t="n"/>
-      <c r="C19" s="48" t="n"/>
-      <c r="D19" s="45" t="n"/>
-      <c r="E19" s="46" t="n"/>
-      <c r="F19" s="48" t="n"/>
-      <c r="G19" s="48" t="n"/>
-      <c r="H19" s="47" t="n"/>
+      <c r="F18" s="33" t="n"/>
+      <c r="G18" s="34" t="n"/>
+      <c r="H18" s="20" t="n"/>
+    </row>
+    <row r="19" ht="18.75" customHeight="1" s="49">
+      <c r="B19" s="6" t="n"/>
+      <c r="C19" s="18" t="n"/>
+      <c r="D19" s="18" t="n"/>
+      <c r="E19" s="19" t="n"/>
+      <c r="F19" s="19" t="n"/>
+      <c r="G19" s="19" t="n"/>
+      <c r="H19" s="19" t="n"/>
     </row>
     <row r="20">
-      <c r="B20" s="52" t="n"/>
-      <c r="C20" s="52" t="n"/>
-      <c r="D20" s="52" t="n"/>
-      <c r="E20" s="52" t="n"/>
-      <c r="F20" s="52" t="n"/>
-      <c r="G20" s="53" t="n"/>
-      <c r="H20" s="52" t="n"/>
-    </row>
-    <row r="21" ht="18.75" customHeight="1" s="65">
-      <c r="B21" s="41" t="n"/>
-      <c r="C21" s="41" t="n"/>
-      <c r="D21" s="41" t="n"/>
-      <c r="E21" s="41" t="n"/>
-      <c r="F21" s="41" t="n"/>
-      <c r="G21" s="51" t="inlineStr">
+      <c r="B20" s="6" t="n"/>
+      <c r="C20" s="18" t="n"/>
+      <c r="D20" s="18" t="n"/>
+      <c r="E20" s="19" t="n"/>
+      <c r="F20" s="19" t="n"/>
+      <c r="G20" s="33" t="n"/>
+      <c r="H20" s="19" t="n"/>
+    </row>
+    <row r="21" ht="18.75" customHeight="1" s="49">
+      <c r="B21" s="6" t="n"/>
+      <c r="C21" s="18" t="n"/>
+      <c r="D21" s="18" t="n"/>
+      <c r="E21" s="19" t="n"/>
+      <c r="F21" s="19" t="n"/>
+      <c r="G21" s="35" t="inlineStr">
         <is>
           <t>Signature</t>
         </is>
       </c>
-      <c r="H21" s="41" t="n"/>
+      <c r="H21" s="19" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>